<commit_message>
Update technology instructor table field.
</commit_message>
<xml_diff>
--- a/Datebase Field.xlsx
+++ b/Datebase Field.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ipst\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="8" activeTab="13"/>
   </bookViews>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4366" uniqueCount="1564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4382" uniqueCount="1568">
   <si>
     <t>เพศ</t>
   </si>
@@ -4724,6 +4729,18 @@
   </si>
   <si>
     <t>h_t_ins_101112_4_4</t>
+  </si>
+  <si>
+    <t>r_t_ins_101112_5_1</t>
+  </si>
+  <si>
+    <t>r_t_ins_101112_5_2</t>
+  </si>
+  <si>
+    <t>t_t_ins_101112_5_3</t>
+  </si>
+  <si>
+    <t>h_t_ins_101112_5_4</t>
   </si>
 </sst>
 </file>
@@ -5115,7 +5132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7920,7 +7937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection sqref="A1:C93"/>
     </sheetView>
   </sheetViews>
@@ -8962,10 +8979,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection sqref="A1:C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9687,6 +9704,50 @@
         <v>1215</v>
       </c>
       <c r="C65" s="14" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>1212</v>
       </c>
     </row>
@@ -15007,10 +15068,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158:B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16121,6 +16182,26 @@
     <row r="157" spans="2:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="11" t="s">
         <v>1563</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="11" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="11" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="11" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="11" t="s">
+        <v>1567</v>
       </c>
     </row>
   </sheetData>
@@ -16207,7 +16288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change request. - Change book display approach in both teacher and student science tab.
</commit_message>
<xml_diff>
--- a/Datebase Field.xlsx
+++ b/Datebase Field.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756"/>
   </bookViews>
   <sheets>
     <sheet name="participant" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4382" uniqueCount="1568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4414" uniqueCount="1600">
   <si>
     <t>เพศ</t>
   </si>
@@ -4741,6 +4741,102 @@
   </si>
   <si>
     <t>h_t_ins_101112_5_4</t>
+  </si>
+  <si>
+    <t>c_sp</t>
+  </si>
+  <si>
+    <t>ฟิสิกส์</t>
+  </si>
+  <si>
+    <t>ฟิสิกส์ ม.4</t>
+  </si>
+  <si>
+    <t>ฟิสิกส์ ม.5</t>
+  </si>
+  <si>
+    <t>ฟิสิกส์ ม.6</t>
+  </si>
+  <si>
+    <t>c_sp_10</t>
+  </si>
+  <si>
+    <t>c_sp_11</t>
+  </si>
+  <si>
+    <t>c_sp_12</t>
+  </si>
+  <si>
+    <t>เคมี</t>
+  </si>
+  <si>
+    <t>เคมี ม.4</t>
+  </si>
+  <si>
+    <t>c_sc</t>
+  </si>
+  <si>
+    <t>c_sc_10</t>
+  </si>
+  <si>
+    <t>c_sc_11</t>
+  </si>
+  <si>
+    <t>c_sc_12</t>
+  </si>
+  <si>
+    <t>เคมี ม.5</t>
+  </si>
+  <si>
+    <t>เคมี ม.6</t>
+  </si>
+  <si>
+    <t>ชีววิทยา</t>
+  </si>
+  <si>
+    <t>ชีววิทยา ม.4</t>
+  </si>
+  <si>
+    <t>ชีววิทยา ม.5</t>
+  </si>
+  <si>
+    <t>ชีววิทยา ม.6</t>
+  </si>
+  <si>
+    <t>c_sb</t>
+  </si>
+  <si>
+    <t>c_sb_10</t>
+  </si>
+  <si>
+    <t>c_sb_11</t>
+  </si>
+  <si>
+    <t>c_sb_12</t>
+  </si>
+  <si>
+    <t>โลก ดาราศาสตร์</t>
+  </si>
+  <si>
+    <t>c_se</t>
+  </si>
+  <si>
+    <t>โลก ดาราศาสตร์ ม.4</t>
+  </si>
+  <si>
+    <t>โลก ดาราศาสตร์ ม.5</t>
+  </si>
+  <si>
+    <t>โลก ดาราศาสตร์ ม.6</t>
+  </si>
+  <si>
+    <t>c_se_10</t>
+  </si>
+  <si>
+    <t>c_se_11</t>
+  </si>
+  <si>
+    <t>c_se_12</t>
   </si>
 </sst>
 </file>
@@ -5140,17 +5236,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="83" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5549,7 +5645,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -5557,7 +5653,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -5565,7 +5661,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -5573,7 +5669,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -5581,7 +5677,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>92</v>
       </c>
@@ -5589,7 +5685,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -5597,7 +5693,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>94</v>
       </c>
@@ -5605,7 +5701,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>95</v>
       </c>
@@ -5613,7 +5709,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -5621,7 +5717,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -5629,7 +5725,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -5637,7 +5733,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -5645,7 +5741,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -5653,7 +5749,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -5661,7 +5757,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -5669,187 +5765,379 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>1569</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>1568</v>
+      </c>
+      <c r="C64" t="str">
+        <f>CONCATENATE("ALTER TABLE `participant` ADD `",B64,"` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT '",A64,"' AFTER `c_d_12`;")</f>
+        <v>ALTER TABLE `participant` ADD `c_sp` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ฟิสิกส์' AFTER `c_d_12`;</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>1570</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" t="s">
-        <v>135</v>
+        <v>1573</v>
+      </c>
+      <c r="C65" t="str">
+        <f>CONCATENATE("ALTER TABLE `participant` ADD `",B65,"` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT '",A65,"' AFTER `",B64,"`;")</f>
+        <v>ALTER TABLE `participant` ADD `c_sp_10` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ฟิสิกส์ ม.4' AFTER `c_sp`;</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>1571</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66" t="s">
-        <v>135</v>
+        <v>1574</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C79" si="0">CONCATENATE("ALTER TABLE `participant` ADD `",B66,"` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT '",A66,"' AFTER `",B65,"`;")</f>
+        <v>ALTER TABLE `participant` ADD `c_sp_11` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ฟิสิกส์ ม.5' AFTER `c_sp_10`;</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>1572</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" t="s">
-        <v>135</v>
+        <v>1575</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sp_12` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ฟิสิกส์ ม.6' AFTER `c_sp_11`;</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>1576</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
-      </c>
-      <c r="C68" t="s">
-        <v>135</v>
+        <v>1578</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sc` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'เคมี' AFTER `c_sp_12`;</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>1577</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" t="s">
-        <v>135</v>
+        <v>1579</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sc_10` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'เคมี ม.4' AFTER `c_sc`;</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>1582</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
-      </c>
-      <c r="C70" t="s">
-        <v>135</v>
+        <v>1580</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sc_11` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'เคมี ม.5' AFTER `c_sc_10`;</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>1583</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
-      </c>
-      <c r="C71" t="s">
-        <v>135</v>
+        <v>1581</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sc_12` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'เคมี ม.6' AFTER `c_sc_11`;</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>1584</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
-      </c>
-      <c r="C72" t="s">
-        <v>135</v>
+        <v>1588</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sb` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ชีววิทยา' AFTER `c_sc_12`;</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>1585</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
-      </c>
-      <c r="C73" t="s">
-        <v>135</v>
+        <v>1589</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sb_10` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ชีววิทยา ม.4' AFTER `c_sb`;</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>754</v>
+        <v>1586</v>
       </c>
       <c r="B74" t="s">
-        <v>755</v>
-      </c>
-      <c r="C74" t="s">
-        <v>756</v>
+        <v>1590</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sb_11` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ชีววิทยา ม.5' AFTER `c_sb_10`;</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>757</v>
+        <v>1587</v>
       </c>
       <c r="B75" t="s">
-        <v>758</v>
-      </c>
-      <c r="C75" t="s">
-        <v>756</v>
+        <v>1591</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_sb_12` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'ชีววิทยา ม.6' AFTER `c_sb_11`;</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>759</v>
+        <v>1592</v>
       </c>
       <c r="B76" t="s">
-        <v>760</v>
-      </c>
-      <c r="C76" t="s">
-        <v>756</v>
+        <v>1593</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_se` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'โลก ดาราศาสตร์' AFTER `c_sb_12`;</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>761</v>
+        <v>1594</v>
       </c>
       <c r="B77" t="s">
-        <v>762</v>
-      </c>
-      <c r="C77" t="s">
-        <v>756</v>
+        <v>1597</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_se_10` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'โลก ดาราศาสตร์ ม.4' AFTER `c_se`;</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>1595</v>
       </c>
       <c r="B78" t="s">
-        <v>763</v>
-      </c>
-      <c r="C78" t="s">
-        <v>756</v>
+        <v>1598</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_se_11` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'โลก ดาราศาสตร์ ม.5' AFTER `c_se_10`;</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>764</v>
+        <v>1596</v>
       </c>
       <c r="B79" t="s">
-        <v>765</v>
-      </c>
-      <c r="C79" t="s">
-        <v>756</v>
+        <v>1599</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE `participant` ADD `c_se_12` CHAR(1) CHARACTER SET utf8 COLLATE utf8_general_ci NULL COMMENT 'โลก ดาราศาสตร์ ม.6' AFTER `c_se_11`;</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" t="s">
+        <v>129</v>
+      </c>
+      <c r="C83" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" t="s">
+        <v>126</v>
+      </c>
+      <c r="C86" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89" t="s">
+        <v>143</v>
+      </c>
+      <c r="C89" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>754</v>
+      </c>
+      <c r="B90" t="s">
+        <v>755</v>
+      </c>
+      <c r="C90" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>757</v>
+      </c>
+      <c r="B91" t="s">
+        <v>758</v>
+      </c>
+      <c r="C91" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>759</v>
+      </c>
+      <c r="B92" t="s">
+        <v>760</v>
+      </c>
+      <c r="C92" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>761</v>
+      </c>
+      <c r="B93" t="s">
+        <v>762</v>
+      </c>
+      <c r="C93" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" t="s">
+        <v>763</v>
+      </c>
+      <c r="C94" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>764</v>
+      </c>
+      <c r="B95" t="s">
+        <v>765</v>
+      </c>
+      <c r="C95" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>150</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B96" t="s">
         <v>148</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C96" t="s">
         <v>149</v>
       </c>
     </row>
@@ -8682,7 +8970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update delete query and fix devide by zero in teacher report.
</commit_message>
<xml_diff>
--- a/Datebase Field.xlsx
+++ b/Datebase Field.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ipst\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="8" activeTab="14"/>
   </bookViews>
@@ -23,7 +28,7 @@
     <sheet name="design_book_instructor" sheetId="13" r:id="rId14"/>
     <sheet name="clear_data" sheetId="16" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4434" uniqueCount="1620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4436" uniqueCount="1622">
   <si>
     <t>เพศ</t>
   </si>
@@ -4893,6 +4898,12 @@
   </si>
   <si>
     <t>ALTER TABLE technology_book_instructor AUTO_INCREMENT = 1;</t>
+  </si>
+  <si>
+    <t>ALTER TABLE design_book AUTO_INCREMENT = 1;</t>
+  </si>
+  <si>
+    <t>DELETE FROM design_book_instructor;</t>
   </si>
 </sst>
 </file>
@@ -5284,7 +5295,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10909,10 +10920,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10947,76 +10958,86 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1605</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1606</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>1619</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Left join contribute in searchQuestionnaireHistory.
</commit_message>
<xml_diff>
--- a/Datebase Field.xlsx
+++ b/Datebase Field.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ipst\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="participant" sheetId="1" r:id="rId1"/>
@@ -27,8 +22,10 @@
     <sheet name="design_book" sheetId="12" r:id="rId13"/>
     <sheet name="design_book_instructor" sheetId="13" r:id="rId14"/>
     <sheet name="clear_data" sheetId="16" r:id="rId15"/>
+    <sheet name="student_book" sheetId="17" r:id="rId16"/>
+    <sheet name="teacher_book" sheetId="18" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4436" uniqueCount="1622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="1678">
   <si>
     <t>เพศ</t>
   </si>
@@ -4904,6 +4901,174 @@
   </si>
   <si>
     <t>DELETE FROM design_book_instructor;</t>
+  </si>
+  <si>
+    <t>วิชาคณิตศาสตร์</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 1</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน</t>
+  </si>
+  <si>
+    <t>แบบฝึกทักษะ เตรียมความพร้อม</t>
+  </si>
+  <si>
+    <t>แบบฝึกทักษะ เล่ม 1</t>
+  </si>
+  <si>
+    <t>แบบฝึกทักษะ เล่ม 2</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 2</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 3</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 4</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 5</t>
+  </si>
+  <si>
+    <t>ชั้นประถมศีกษาปีที่ 6</t>
+  </si>
+  <si>
+    <t>ชั้นมัธยมศึกษาปีที่ 1</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาพื้นฐาน เล่ม 1</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาพื้นฐาน เล่ม 2</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 1</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 2</t>
+  </si>
+  <si>
+    <t>ชั้นมัธยมศึกษาปีที่ 2</t>
+  </si>
+  <si>
+    <t>ชั้นมัธยมศึกษาปีที่ 3</t>
+  </si>
+  <si>
+    <t>ชั้นมัธยมศึกษาปีที่ 4-6</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาพื้นฐาน เล่ม 3</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 3</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 4</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 5</t>
+  </si>
+  <si>
+    <t>หนังสือเรียน รายวิชาเพิ่มเติม เล่ม 6</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>คู่มือครูวิชาวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาพื้นฐาน</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาพื้นฐาน เล่ม 1</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาพื้นฐาน เล่ม 2</t>
+  </si>
+  <si>
+    <t>ชั้นมัธยมศึกษาปีที่ 1-3</t>
+  </si>
+  <si>
+    <t>คู่มือครู เชื้อเพลิงเพื่อการคมนาคม</t>
+  </si>
+  <si>
+    <t>คู่มือครู ของเล่นเชิงวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>คู่มือครู วิทยาศาสตร์กับความงาม</t>
+  </si>
+  <si>
+    <t>คู่มือครู สนุกกับโครงงานวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>คู่มือครู พลังงานทดแทนกับการใช้ประโยชน์</t>
+  </si>
+  <si>
+    <t>คู่มือครู การเคลื่อนที่และแรงในธรรมชาติ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">วิทยาศาสตร์ สำหรับนักเรียนที่ไม่เน้นวิทยาศาสตร์ </t>
+  </si>
+  <si>
+    <t>คู่มือครู ดวงดาวและโลกของเรา</t>
+  </si>
+  <si>
+    <t>คู่มือครู พลังงาน</t>
+  </si>
+  <si>
+    <t>คู่มือครู พันธุกรรมและสิ่งแวดล้อม</t>
+  </si>
+  <si>
+    <t>คู่มือครู สารและสมบัติของสาร</t>
+  </si>
+  <si>
+    <t>คู่มือครู ดุลยภาพของสิ่งมีชีวิต</t>
+  </si>
+  <si>
+    <t>ฟิสิกส์ สำหรับนักเรียนที่เน้นวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาเพิ่มเติม เล่ม 1</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาเพิ่มเติม เล่ม 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">คู่มือครู รายวิชาเพิ่มเติม เล่ม 3 </t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาเพิ่มเติม เล่ม 4</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาเพิ่มเติม เล่ม 5</t>
+  </si>
+  <si>
+    <t>เคมี สำหรับนักเรียนที่เน้นวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>คู่มือครู รายวิชาเพิ่มเติม เล่ม 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">คู่มือครู รายวิชาเพิ่มเติม เล่ม 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">คู่มือครู รายวิชาเพิ่มเติม เล่ม 5 </t>
+  </si>
+  <si>
+    <t>ชีววิทยา สำหรับนักเรียนที่เน้นวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>โลก ดาราศาสตร์ และอวกาศ สำหรับนักเรียนที่เน้นวิทยาศาสตร์</t>
   </si>
 </sst>
 </file>
@@ -5295,7 +5460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10922,7 +11087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -11039,6 +11204,826 @@
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1619</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>445</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>452</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>464</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>480</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>484</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>488</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>508</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>512</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>516</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>584</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>536</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>540</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>544</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>580</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>548</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>552</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>556</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>576</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>767</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>774</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>778</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>782</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>786</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>830</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>834</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>838</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>842</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>846</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>850</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>854</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>858</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>862</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>866</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>870</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fig bug. prevent resubmit with refresh.
</commit_message>
<xml_diff>
--- a/Datebase Field.xlsx
+++ b/Datebase Field.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="10" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" tabRatio="756" firstSheet="11" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="participant" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="clear_data" sheetId="16" r:id="rId15"/>
     <sheet name="student_book" sheetId="17" r:id="rId16"/>
     <sheet name="teacher_book" sheetId="18" r:id="rId17"/>
+    <sheet name="delete by id" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="1678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="1688">
   <si>
     <t>เพศ</t>
   </si>
@@ -5069,6 +5070,36 @@
   </si>
   <si>
     <t>โลก ดาราศาสตร์ และอวกาศ สำหรับนักเรียนที่เน้นวิทยาศาสตร์</t>
+  </si>
+  <si>
+    <t>delete from contribute where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from design_book where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from design_book_instructor where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from math_book where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from math_book_instructor where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from science_book where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from science_book_instructor where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from technology_book where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from technology_book_instructor where id = 3669;</t>
+  </si>
+  <si>
+    <t>delete from participant where id = 3669;</t>
   </si>
 </sst>
 </file>
@@ -5460,7 +5491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11590,8 +11621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12024,6 +12055,74 @@
       </c>
       <c r="C47" t="s">
         <v>1673</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>